<commit_message>
add stock market story
</commit_message>
<xml_diff>
--- a/jupyter/location.xlsx
+++ b/jupyter/location.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hr\jupyter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E0C1F3-5B83-4D21-B08A-A026721228C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F140FC-D9AF-4C2E-8166-B119FE5FF771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{38A53CF7-E57B-4F46-AD7B-56FC794CE2F9}"/>
   </bookViews>
@@ -280,7 +280,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="183" formatCode="_-* #,##0.00000000_-;\-* #,##0.00000000_-;_-* &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -291,6 +295,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
@@ -320,23 +332,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="쉼표 [0]" xfId="1" builtinId="6"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="183" formatCode="_-* #,##0.00000000_-;\-* #,##0.00000000_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="183" formatCode="_-* #,##0.00000000_-;\-* #,##0.00000000_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -357,8 +383,8 @@
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{DEE8150C-235F-4A7A-8E02-48CB358E1302}" name="근무지"/>
-    <tableColumn id="2" xr3:uid="{9B2AECD8-D39A-4C68-8126-CB100F26968D}" name="위도"/>
-    <tableColumn id="3" xr3:uid="{85A5762D-96C1-4FD9-9773-3B75CB24FBFF}" name="경도"/>
+    <tableColumn id="2" xr3:uid="{9B2AECD8-D39A-4C68-8126-CB100F26968D}" name="위도" dataDxfId="1" dataCellStyle="쉼표 [0]"/>
+    <tableColumn id="3" xr3:uid="{85A5762D-96C1-4FD9-9773-3B75CB24FBFF}" name="경도" dataDxfId="0" dataCellStyle="쉼표 [0]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -664,7 +690,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -688,10 +714,10 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>37.376923024352301</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>127.106107697859</v>
       </c>
     </row>
@@ -699,10 +725,10 @@
       <c r="A3" t="s">
         <v>72</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>37.364095900000002</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>127.000353</v>
       </c>
     </row>
@@ -710,10 +736,10 @@
       <c r="A4" t="s">
         <v>75</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>37.378442</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>127.21423</v>
       </c>
     </row>
@@ -721,10 +747,10 @@
       <c r="A5" t="s">
         <v>70</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>37.306574444503198</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>127.137412074906</v>
       </c>
     </row>
@@ -732,10 +758,10 @@
       <c r="A6" t="s">
         <v>76</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>37.486460899999997</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>126.6298197</v>
       </c>
     </row>
@@ -743,10 +769,10 @@
       <c r="A7" t="s">
         <v>73</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>37.486460899999997</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>126.6298197</v>
       </c>
     </row>
@@ -754,10 +780,10 @@
       <c r="A8" t="s">
         <v>57</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>37.285314999999997</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>126.8882818</v>
       </c>
     </row>
@@ -765,10 +791,10 @@
       <c r="A9" t="s">
         <v>67</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>35.5057777899586</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>129.44174303901499</v>
       </c>
     </row>
@@ -776,10 +802,10 @@
       <c r="A10" t="s">
         <v>69</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>35.946756301741999</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>129.26716099999999</v>
       </c>
     </row>
@@ -787,10 +813,10 @@
       <c r="A11" t="s">
         <v>68</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>35.969776970996598</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>126.59654233664899</v>
       </c>
     </row>
@@ -798,10 +824,10 @@
       <c r="A12" t="s">
         <v>74</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>35.967714299999997</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>126.5800686</v>
       </c>
     </row>
@@ -809,10 +835,10 @@
       <c r="A13" t="s">
         <v>49</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>36.285188300000002</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>126.6371552</v>
       </c>
     </row>
@@ -820,10 +846,10 @@
       <c r="A14" t="s">
         <v>77</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="2">
         <v>36.931209500000001</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>127.752218</v>
       </c>
     </row>
@@ -841,7 +867,7 @@
   <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:G3"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>